<commit_message>
resultats arimafd en multivarié
</commit_message>
<xml_diff>
--- a/merlin_abnormal_multivariate_point_results.xlsx
+++ b/merlin_abnormal_multivariate_point_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,22 +466,42 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>iforestASD_identified</t>
+          <t>MILOF_identified</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>iforestASD_Overlap_merlin</t>
+          <t>MILOF_Overlap_merlin</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>iforestASDbest_param</t>
+          <t>MILOFbest_param</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>iforestASDtime_taken</t>
+          <t>MILOFtime_taken</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ARIMAFD_identified</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ARIMAFD_Overlap_merlin</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ARIMAFDbest_param</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ARIMAFDtime_taken</t>
         </is>
       </c>
     </row>
@@ -512,19 +532,35 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967]</t>
+          <t>[88, 552, 797, 825]</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>{'window_size': 222, 'n_estimator': 12}</t>
+          <t>{'Numk': 14, 'KPar': 11, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.0005128769989823923</v>
+        <v>9.049631076006335</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>[133, 464, 628, 963]</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>{'window_size': 92}</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>1188.046888874</v>
       </c>
     </row>
     <row r="3">
@@ -554,7 +590,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[135, 158, 214, 253]</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -562,11 +598,27 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 10, 'KPar': 13, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>11.40097611300007</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>[314, 325, 684, 968]</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>{'window_size': 181}</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>5028.996044122003</v>
       </c>
     </row>
     <row r="4">
@@ -596,7 +648,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[202, 227, 295, 372]</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -604,11 +656,27 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 9, 'KPar': 11, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>10.41810625100334</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>[181, 190, 583, 597]</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>{'window_size': 123}</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>265.9657750680053</v>
       </c>
     </row>
     <row r="5">
@@ -638,7 +706,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[175, 312]</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -646,11 +714,27 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 11, 'KPar': 5, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J5" t="n">
+        <v>6.335740316993906</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>[503, 745]</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
         <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>{'window_size': 176}</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>3866.292378414015</v>
       </c>
     </row>
     <row r="6">
@@ -680,7 +764,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[372, 383]</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -688,11 +772,27 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 10, 'KPar': 3, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>5.555181247997098</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>[203, 987]</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>{'window_size': 203}</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>4814.967263817991</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +822,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[58, 64, 528, 536]</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -730,11 +830,27 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 6, 'KPar': 6, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>5.160258635005448</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>[104, 155, 194, 199]</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>{'window_size': 90}</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>962.8695973639842</v>
       </c>
     </row>
     <row r="8">
@@ -764,7 +880,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[177, 787, 958, 1068]</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -772,11 +888,27 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 14, 'KPar': 5, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>5.478524310994544</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>[435, 444, 571, 628]</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>{'window_size': 268}</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>8245.638174999011</v>
       </c>
     </row>
     <row r="9">
@@ -806,7 +938,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>[443, 798, 806, 810, 823]</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -814,114 +946,27 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>params</t>
+          <t>{'Numk': 12, 'KPar': 11, 'Bucket_index': 500}</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>clean_multivariate/creditcard.csv</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>284807</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>creditcard</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>492</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   541;    623;   4920;   6108;   6329;   6331;   6334;   6336;
-         6338;   6427;   6446;   6472;   6529;   6609;   6641;   6717;
-         6719;   6734;   6774;   6820;   6870;   6882;   6899;   6903;
-         6971;   8296;   8312;   8335;   8615;   8617;   8842;   8845;
-         8972;   9035;   9179;   9252;   9487;   9509;  10204;  10484;
-        10497;  10498;  10568;  10630;  10690;  10801;  10891;  10897;
-        11343;  11710;  11841;  11880;  12070;  12108;  12261;  12369;
-        14104;  14170;  14197;  14211;  14338;  15166;  15204;  15225;
-        15451;  15476;  15506;  15539;  15566;  15736;  15751;  15781;
-        15810;  16415;  16780;  16863;  17317;  17366;  17407;  17453;
-        17480;  18466;  18472;  18773;  18809;  20198;  23308;  23422;
-        26802;  27362;  27627;  27738;  27749;  29687;  30100;  30314;
-        30384;  30398;  30442;  30473;  30496;  31002;  33276;  39183;
-        40085;  40525;  41395;  41569;  41943;  42007;  42009;  42473;
-        42528;  42549;  42590;  42609;  42635;  42674;  42696;  42700;
-        42741;  42756;  42769;  42784;  42856;  42887;  42936;  42945;
-        42958;  43061;  43160;  43204;  43428;  43624;  43681;  43773;
-        44001;  44091;  44223;  44270;  44556;  45203;  45732;  46909;
-        46918;  46998;  47802;  48094;  50211;  50537;  52466;  52521;
-        52584;  53591;  53794;  55401;  56703;  57248;  57470;  57615;
-        58422;  58761;  59539;  61787;  63421;  63634;  64329;  64411;
-        64460;  68067;  68320;  68522;  68633;  69498;  69980;  70141;
-        70589;  72757;  73784;  73857;  74496;  74507;  74794;  75511;
-        76555;  76609;  76929;  77099;  77348;  77387;  77682;  79525;
-        79536;  79835;  79874;  79883;  80760;  81186;  81609;  82400;
-        83053;  83297;  83417;  84543;  86155;  87354;  88258;  88307;
-        88876;  88897;  89190;  91671;  92777;  93424;  93486;  93788;
-        94218;  95534;  95597;  96341;  96789;  96994;  99506; 100623;
-       101509; 102441; 102442; 102443; 102444; 102445; 102446; 102782;
-       105178; 106679; 106998; 107067; 107637; 108258; 108708; 111690;
-       112840; 114271; 116139; 116404; 118308; 119714; 119781; 120505;
-       120837; 122479; 123141; 123201; 123238; 123270; 123301; 124036;
-       124087; 124115; 124176; 125342; 128479; 131272; 135718; 137705;
-       140786; 141257; 141258; 141259; 141260; 142405; 142557; 143188;
-       143333; 143334; 143335; 143336; 143728; 143731; 144104; 144108;
-       144754; 145800; 146790; 147548; 147605; 149145; 149357; 149522;
-       149577; 149587; 149600; 149869; 149874; 150601; 150644; 150647;
-       150654; 150660; 150661; 150662; 150663; 150665; 150666; 150667;
-       150668; 150669; 150677; 150678; 150679; 150680; 150684; 150687;
-       150692; 150697; 150715; 150925; 151006; 151007; 151008; 151009;
-       151011; 151103; 151196; 151462; 151519; 151730; 151807; 152019;
-       152223; 152295; 153823; 153835; 153885; 154234; 154286; 154371;
-       154454; 154587; 154633; 154668; 154670; 154676; 154684; 154693;
-       154694; 154697; 154718; 154719; 154720; 154960; 156988; 156990;
-       157585; 157868; 157871; 157918; 163149; 163586; 167184; 167305;
-       172787; 176049; 177195; 178208; 181966; 182992; 183106; 184379;
-       189587; 189701; 189878; 190368; 191074; 191267; 191359; 191544;
-       191690; 192382; 192529; 192584; 192687; 195383; 197586; 198868;
-       199896; 201098; 201601; 203324; 203328; 203700; 204064; 204079;
-       204503; 208651; 212516; 212644; 213092; 213116; 214662; 214775;
-       215132; 215953; 215984; 218442; 219025; 219892; 220725; 221018;
-       221041; 222133; 222419; 223366; 223572; 223578; 223618; 226814;
-       226877; 229712; 229730; 230076; 230476; 231978; 233258; 234574;
-       234632; 234633; 234705; 235616; 235634; 235644; 237107; 237426;
-       238222; 238366; 238466; 239499; 239501; 240222; 241254; 241445;
-       243393; 243547; 243699; 243749; 243848; 244004; 244333; 245347;
-       245556; 247673; 247995; 248296; 248971; 249167; 249239; 249607;
-       249828; 249963; 250761; 251477; 251866; 251881; 251891; 251904;
-       252124; 252774; 254344; 254395; 255403; 255556; 258403; 261056;
-       261473; 261925; 262560; 262826; 263080; 263274; 263324; 263877;
-       268375; 272521; 274382; 274475; 275992; 276071; 276864; 279863;
-       280143; 280149; 281144; 281674</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>params</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
+        <v>10.42844949501159</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>[148, 178, 787, 980]</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>{'window_size': 148}</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>1719.089206571982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
score kitnet dans abnormal multivariate
</commit_message>
<xml_diff>
--- a/merlin_abnormal_multivariate_point_results.xlsx
+++ b/merlin_abnormal_multivariate_point_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,26 @@
           <t>ARIMAFDtime_taken</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>KitNet_identified</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>KitNet_Overlap_merlin</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>KitNetbest_param</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>KitNettime_taken</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -562,6 +582,22 @@
       <c r="N2" t="n">
         <v>1188.046888874</v>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967]</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>{'window_size': 957}</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>0.01320189400576055</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -620,6 +656,22 @@
       <c r="N3" t="n">
         <v>5028.996044122003</v>
       </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>[543, 544, 545, 551, 553, 556, 562, 633, 1100]</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>{'window_size': 542}</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>0.1108410270535387</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -678,6 +730,22 @@
       <c r="N4" t="n">
         <v>265.9657750680053</v>
       </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>[933, 934, 935, 936, 939, 940, 943, 945, 989, 1024]</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>{'window_size': 932}</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>0.05484268598956987</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -736,6 +804,22 @@
       <c r="N5" t="n">
         <v>3866.292378414015</v>
       </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750]</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>{'window_size': 759}</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
+        <v>0.008580877038184553</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -794,6 +878,22 @@
       <c r="N6" t="n">
         <v>4814.967263817991</v>
       </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>[266, 579]</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>{'window_size': 265}</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
+        <v>0.1128086459939368</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -852,6 +952,22 @@
       <c r="N7" t="n">
         <v>962.8695973639842</v>
       </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664]</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>{'window_size': 839}</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>0.01477298198733479</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -910,6 +1026,22 @@
       <c r="N8" t="n">
         <v>8245.638174999011</v>
       </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>[626, 627, 628, 629, 630, 632, 636, 638, 840, 1066, 1067, 1068, 1069, 1070, 1072, 1075]</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>{'window_size': 625}</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
+        <v>0.08223781501874328</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -954,19 +1086,35 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[148, 178, 787, 980]</t>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146]</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{'window_size': 148}</t>
+          <t>{'window_size': 131}</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>1719.089206571982</v>
+        <v>9.502982720732689e-06</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>[872, 873, 874, 876, 877, 878, 879, 885, 886, 887, 889, 890, 891, 893, 894, 895, 898, 907, 985]</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>{'window_size': 871}</t>
+        </is>
+      </c>
+      <c r="R9" t="n">
+        <v>0.06458198599284515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
online arima en univarié en cours
</commit_message>
<xml_diff>
--- a/merlin_abnormal_multivariate_point_results.xlsx
+++ b/merlin_abnormal_multivariate_point_results.xlsx
@@ -648,11 +648,11 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>{'window_size': 226, 'n_estimator': 24}</t>
+          <t>{'max_features': 1, 'window_size': 226, 'n_estimator': 15}</t>
         </is>
       </c>
       <c r="V2" t="n">
-        <v>39.68085051898379</v>
+        <v>42.76856716792099</v>
       </c>
       <c r="W2" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>[863, 934, 954, 1068]</t>
+          <t>[863, 866, 934, 954, 1068]</t>
         </is>
       </c>
       <c r="T3" t="n">
@@ -754,11 +754,11 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>{'window_size': 245, 'n_estimator': 18}</t>
+          <t>{'max_features': 2, 'window_size': 251, 'n_estimator': 45}</t>
         </is>
       </c>
       <c r="V3" t="n">
-        <v>31.91015833697747</v>
+        <v>54.92935482901521</v>
       </c>
       <c r="W3" t="inlineStr">
         <is>
@@ -852,7 +852,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>[832, 862, 873, 1046]</t>
+          <t>[832, 852, 862, 868, 873]</t>
         </is>
       </c>
       <c r="T4" t="n">
@@ -860,11 +860,11 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>{'window_size': 273, 'n_estimator': 30}</t>
+          <t>{'max_features': 3, 'window_size': 202, 'n_estimator': 29}</t>
         </is>
       </c>
       <c r="V4" t="n">
-        <v>31.33925589901628</v>
+        <v>58.2047609569272</v>
       </c>
       <c r="W4" t="inlineStr">
         <is>
@@ -966,11 +966,11 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>{'window_size': 200, 'n_estimator': 33}</t>
+          <t>{'max_features': 6, 'window_size': 200, 'n_estimator': 38}</t>
         </is>
       </c>
       <c r="V5" t="n">
-        <v>32.99023232195759</v>
+        <v>35.67835730698425</v>
       </c>
       <c r="W5" t="inlineStr">
         <is>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>[824, 991]</t>
+          <t>[963, 991]</t>
         </is>
       </c>
       <c r="T6" t="n">
@@ -1072,11 +1072,11 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>{'window_size': 205, 'n_estimator': 26}</t>
+          <t>{'max_features': 2, 'window_size': 254, 'n_estimator': 17}</t>
         </is>
       </c>
       <c r="V6" t="n">
-        <v>32.02282776898937</v>
+        <v>55.26876066299155</v>
       </c>
       <c r="W6" t="inlineStr">
         <is>
@@ -1178,11 +1178,11 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>{'window_size': 200, 'n_estimator': 18}</t>
+          <t>{'max_features': 4, 'window_size': 200, 'n_estimator': 24}</t>
         </is>
       </c>
       <c r="V7" t="n">
-        <v>30.90617852198193</v>
+        <v>33.94053089502268</v>
       </c>
       <c r="W7" t="inlineStr">
         <is>
@@ -1276,19 +1276,19 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>[1, 248, 268, 850]</t>
+          <t>[1, 248, 268, 827]</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>{'window_size': 249, 'n_estimator': 27}</t>
+          <t>{'max_features': 3, 'window_size': 240, 'n_estimator': 23}</t>
         </is>
       </c>
       <c r="V8" t="n">
-        <v>36.3180539769819</v>
+        <v>61.38626400299836</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
@@ -1382,19 +1382,19 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>[836, 892, 919, 984]</t>
+          <t>[813, 892, 984, 1026]</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>{'window_size': 206, 'n_estimator': 24}</t>
+          <t>{'max_features': 6, 'window_size': 213, 'n_estimator': 30}</t>
         </is>
       </c>
       <c r="V9" t="n">
-        <v>32.10083238501102</v>
+        <v>55.47462417802308</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>

</xml_diff>